<commit_message>
files used for herbicide BEs
</commit_message>
<xml_diff>
--- a/ESA_script_tracker.xlsx
+++ b/ESA_script_tracker.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JConno02\Documents\GitHub\ESA_Scripts_Fall2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JConno02\Documents\GitHub\ESA_Species\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F683DE-114E-477E-B078-15B1A87D1E21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
@@ -19,7 +20,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ESA_script_tracker!$A$1:$C$131</definedName>
   </definedNames>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -944,7 +952,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1966,15 +1974,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2327,12 +2333,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2647,7 +2653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView topLeftCell="A97" workbookViewId="0">
@@ -4102,7 +4108,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C131"/>
+  <autoFilter ref="A1:C131" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="597" r:id="rId1"/>

</xml_diff>